<commit_message>
Update Create Responsive Search Ad(s).xlsx
</commit_message>
<xml_diff>
--- a/_posts/도서/마케팅/file/Create Responsive Search Ad(s).xlsx
+++ b/_posts/도서/마케팅/file/Create Responsive Search Ad(s).xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhine/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\study\shina1221.github.io\_posts\도서\마케팅\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD4B15-022D-C743-8976-BE3EC20D2767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="(Template) Create RSA" sheetId="1" r:id="rId1"/>
-    <sheet name="(Example) Create RSA" sheetId="2" r:id="rId2"/>
-    <sheet name="(Example 2) Create RSA" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="(Example) Create RSA" sheetId="2" r:id="rId3"/>
+    <sheet name="(Example 2) Create RSA" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="231">
   <si>
     <t xml:space="preserve">#Optional.
 </t>
@@ -504,12 +504,1438 @@
   <si>
     <t>https://m.example.com</t>
   </si>
+  <si>
+    <r>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d Status(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>ㄱ</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>베어</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의류</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>엑세서리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일반</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의류</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>티셔츠</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의류</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>청바지</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>샌들</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신발</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>운동화</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>액세서리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>모자</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>베어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>액세서리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가방</t>
+    </r>
+  </si>
+  <si>
+    <t>Responsive search ad</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">첫 구매시 10% 할인 </t>
+  </si>
+  <si>
+    <t>베어 - 흰다</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 신상품 입고</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다 신상품 입고</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>럭셔리 플랫폼</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>뉴 시즌 디자이너 컬렉션</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>의류</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>신발</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>액세서리</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>티셔츠</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>청바지</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>샌들</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>운동화</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>모자</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시즌</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>디자이너</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가방</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금 구매하기</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감 임박</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>컬렉션 한정</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>첫 구매시 11% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 12% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 13% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 14% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 15% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 16% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 17% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 18% 할인</t>
+  </si>
+  <si>
+    <t>첫 구매시 19% 할인</t>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 의류 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 신발 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 액세서리 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 티셔츠 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 청바지 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 샌들 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 운동화 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 모자 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 가방 컬렉션을 지금 구매하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 의류 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 신발 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 액세서리 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 티셔츠 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 청바지 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 샌들 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 운동화 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 모자 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 가방 컬렉션을 지금 확인하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 의류 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 신발 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 액세서리 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 티셔츠 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 청바지 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 샌들 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 운동화 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 모자 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 가방 컬렉션을 지금 신청하세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>컬렉션</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>의류</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>신발</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>액세서리</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>티셔츠</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>청바지</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>샌들</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동화</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>모자</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>가방</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear/clothing</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear/shoes</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear/accessories</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear/t-shirts</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear/t-shirts/bear-woofie-t-shirts</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.heenda.com/designer/bear/jeans</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 모자</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 디자이너</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 의류</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 신발</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 액세서리</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 티셔츠</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 청바지</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 샌들</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 운동화</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 가방</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>베어 디자이너 입점</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">베어 따끈한 신상품 입고 </t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>흰다에서 새로운 베어 디자이너 컬렉션을 지금 뽑으세요</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>전 상품 무료배송 및 무료반품</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>디자이너 단독 컬렉션 입점 중</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>신상품 매일 입고</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>전 상품 무료배송 및 무료 반품</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>디자이너 단독 컬렉션 입점 중</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>신상품 매일 입고</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -546,6 +1972,39 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="D2Coding"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -570,10 +2029,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -590,21 +2050,28 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -816,43 +2283,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BB3"/>
+  <dimension ref="A1:BB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BA22" sqref="BA22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.5" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="27.5" customWidth="1"/>
-    <col min="9" max="9" width="45.1640625" customWidth="1"/>
-    <col min="10" max="10" width="30.1640625" customWidth="1"/>
-    <col min="11" max="18" width="22.33203125" customWidth="1"/>
-    <col min="19" max="24" width="22.5" customWidth="1"/>
-    <col min="25" max="28" width="23.5" customWidth="1"/>
-    <col min="29" max="43" width="23.1640625" customWidth="1"/>
-    <col min="44" max="46" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="45.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="11" max="18" width="22.28515625" customWidth="1"/>
+    <col min="19" max="24" width="22.42578125" customWidth="1"/>
+    <col min="25" max="28" width="23.42578125" customWidth="1"/>
+    <col min="29" max="43" width="23.140625" customWidth="1"/>
+    <col min="44" max="46" width="22.28515625" customWidth="1"/>
     <col min="47" max="47" width="34" customWidth="1"/>
-    <col min="48" max="49" width="22.33203125" customWidth="1"/>
-    <col min="50" max="50" width="45.5" customWidth="1"/>
-    <col min="51" max="51" width="40.33203125" customWidth="1"/>
-    <col min="52" max="52" width="61.6640625" customWidth="1"/>
-    <col min="53" max="53" width="22.33203125" customWidth="1"/>
-    <col min="54" max="54" width="33.6640625" customWidth="1"/>
+    <col min="48" max="49" width="22.28515625" customWidth="1"/>
+    <col min="50" max="50" width="45.42578125" customWidth="1"/>
+    <col min="51" max="51" width="40.28515625" customWidth="1"/>
+    <col min="52" max="52" width="61.7109375" customWidth="1"/>
+    <col min="53" max="53" width="22.28515625" customWidth="1"/>
+    <col min="54" max="54" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="11" customFormat="1" ht="131" customHeight="1">
+    <row r="1" spans="1:54" s="9" customFormat="1" ht="131.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -862,10 +2329,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
@@ -950,7 +2417,7 @@
       <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AH1" s="8" t="s">
         <v>31</v>
       </c>
       <c r="AI1" s="2" t="s">
@@ -1014,7 +2481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:54" ht="15">
       <c r="A2" s="4" t="s">
         <v>52</v>
       </c>
@@ -1178,24 +2645,1819 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:54">
-      <c r="A3" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>107</v>
+    <row r="3" spans="1:54" ht="15">
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AV3" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="AW3" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="AX3" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="U4" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X4" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y4" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB4" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW4" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="AX4" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R5" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="U5" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V5" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W5" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y5" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA5" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB5" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AV5" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW5" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX5" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V6" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AV6" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW6" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="AX6" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="U7" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W7" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X7" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y7" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA7" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB7" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW7" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="AX7" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z8" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA8" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB8" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AV8" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW8" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="AX8" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="U9" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X9" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y9" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z9" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA9" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB9" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AV9" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW9" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX9" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="U10" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V10" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W10" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y10" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z10" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA10" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB10" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AV10" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW10" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="AX10" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T11" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="U11" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W11" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y11" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z11" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AV11" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW11" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX11" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" ht="15.75" customHeight="1">
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="N12" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S12" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="U12" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V12" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W12" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X12" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y12" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z12" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA12" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB12" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AV12" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AW12" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="AX12" s="15" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="AX3" r:id="rId1"/>
+    <hyperlink ref="AX4" r:id="rId2"/>
+    <hyperlink ref="AX7" r:id="rId3"/>
+    <hyperlink ref="AX8" r:id="rId4"/>
+    <hyperlink ref="AX12" r:id="rId5"/>
+    <hyperlink ref="AX11" r:id="rId6"/>
+    <hyperlink ref="AX10" r:id="rId7"/>
+    <hyperlink ref="AX9" r:id="rId8"/>
+    <hyperlink ref="AX5" r:id="rId9"/>
+    <hyperlink ref="AX6" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB2" sqref="J2:AB11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="15">
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="15">
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF3" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15">
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="U4" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X4" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y4" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="AB4" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE4" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF4" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="15">
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R5" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="U5" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V5" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W5" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y5" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z5" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="AA5" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB5" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE5" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF5" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="15">
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R6" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T6" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="U6" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V6" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W6" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE6" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF6" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="15">
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q7" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R7" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S7" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="U7" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W7" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X7" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y7" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="AA7" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB7" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE7" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF7" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="15">
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y8" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z8" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA8" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB8" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC8">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE8" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AF8" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="15">
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N9" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="U9" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W9" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X9" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y9" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z9" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA9" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="AB9" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE9" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF9" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="15">
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q10" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="U10" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V10" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W10" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y10" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z10" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="AA10" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="AB10" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC10">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE10" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF10" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="15">
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q11" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="T11" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="U11" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="W11" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="X11" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y11" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z11" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB11" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC11">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="AE11" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF11" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="AF2" r:id="rId1"/>
+    <hyperlink ref="AF3" r:id="rId2"/>
+    <hyperlink ref="AF6" r:id="rId3"/>
+    <hyperlink ref="AF7" r:id="rId4"/>
+    <hyperlink ref="AF11" r:id="rId5"/>
+    <hyperlink ref="AF10" r:id="rId6"/>
+    <hyperlink ref="AF9" r:id="rId7"/>
+    <hyperlink ref="AF8" r:id="rId8"/>
+    <hyperlink ref="AF4" r:id="rId9"/>
+    <hyperlink ref="AF5" r:id="rId10"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1203,22 +4465,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="7" max="8" width="30.1640625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
-    <col min="12" max="12" width="45.5" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1256,7 +4518,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>106</v>
       </c>
@@ -1295,38 +4557,39 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="8" width="30.1640625" customWidth="1"/>
-    <col min="9" max="9" width="22.33203125" customWidth="1"/>
-    <col min="10" max="11" width="23.5" customWidth="1"/>
-    <col min="12" max="13" width="26.33203125" customWidth="1"/>
-    <col min="14" max="15" width="45.5" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="11" width="23.42578125" customWidth="1"/>
+    <col min="12" max="13" width="26.28515625" customWidth="1"/>
+    <col min="14" max="15" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
@@ -1373,7 +4636,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>106</v>
       </c>
@@ -1420,11 +4683,18 @@
         <v>122</v>
       </c>
     </row>
+    <row r="68" spans="3:3" ht="15.75" customHeight="1">
+      <c r="C68" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="O2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="N2" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>